<commit_message>
This is a sample proj plan (basic)
 Basic plan
</commit_message>
<xml_diff>
--- a/AB_Activity-Template_-Gantt-chart.xlsx
+++ b/AB_Activity-Template_-Gantt-chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anandabhaumik/binmon/projectManagement/GoogleProjectManagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45635670-78FE-1D4A-89C7-BDC3654B01D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF874470-01E1-4D48-9682-DA0244741893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,7 @@
         <sz val="10"/>
         <color rgb="FF34A853"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">TITLE: </t>
     </r>
@@ -51,6 +52,7 @@
         <sz val="11"/>
         <color rgb="FF666666"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Plant Pals Operations and Training Plan</t>
     </r>
@@ -68,6 +70,7 @@
         <sz val="10"/>
         <color rgb="FF34A853"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>PROJECT MANAGER:</t>
     </r>
@@ -77,6 +80,7 @@
         <sz val="10"/>
         <color rgb="FF666666"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -86,6 +90,7 @@
         <sz val="11"/>
         <color rgb="FF666666"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>[Name]</t>
     </r>
@@ -100,9 +105,6 @@
     <t>TASK ID NUMBER</t>
   </si>
   <si>
-    <t>MILESTONES &amp; TASKS</t>
-  </si>
-  <si>
     <t>TASK OWNER</t>
   </si>
   <si>
@@ -308,6 +310,9 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILESTONES &amp; TASKS </t>
   </si>
 </sst>
 </file>
@@ -327,155 +332,183 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="30"/>
       <color rgb="FF0B5394"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF0B5394"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="30"/>
       <color rgb="FF34A853"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="29"/>
       <color rgb="FF34A853"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="30"/>
       <color rgb="FF38761D"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF34A853"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF999999"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF073763"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF073763"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF434343"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF434343"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF434343"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -791,11 +824,29 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -804,7 +855,6 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -812,28 +862,11 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1096,7 +1129,7 @@
   <dimension ref="A1:CE973"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C13" sqref="C13:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -1281,30 +1314,30 @@
     </row>
     <row r="7" spans="1:83" ht="37" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
-      <c r="S7" s="75"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="62"/>
-      <c r="V7" s="62"/>
-      <c r="W7" s="62"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="65"/>
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
@@ -1452,34 +1485,34 @@
     </row>
     <row r="9" spans="1:83" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="66" t="s">
+      <c r="I9" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="77" t="s">
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="62"/>
-      <c r="W9" s="62"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="65"/>
+      <c r="W9" s="65"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -1543,34 +1576,34 @@
     </row>
     <row r="10" spans="1:83" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="66" t="s">
+      <c r="I10" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="68" t="s">
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+      <c r="N10" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
-      <c r="T10" s="62"/>
-      <c r="U10" s="62"/>
-      <c r="V10" s="62"/>
-      <c r="W10" s="62"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
+      <c r="U10" s="65"/>
+      <c r="V10" s="65"/>
+      <c r="W10" s="65"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
@@ -1804,235 +1837,235 @@
     </row>
     <row r="13" spans="1:83" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="18"/>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="78" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="E13" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="71" t="s">
+      <c r="F13" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="71" t="s">
+      <c r="G13" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="71" t="s">
+      <c r="H13" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="71" t="s">
+      <c r="I13" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="72" t="s">
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="65"/>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="65"/>
+      <c r="S13" s="65"/>
+      <c r="T13" s="65"/>
+      <c r="U13" s="65"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="65"/>
+      <c r="X13" s="65"/>
+      <c r="Y13" s="65"/>
+      <c r="Z13" s="65"/>
+      <c r="AA13" s="65"/>
+      <c r="AB13" s="65"/>
+      <c r="AC13" s="65"/>
+      <c r="AD13" s="65"/>
+      <c r="AE13" s="65"/>
+      <c r="AF13" s="65"/>
+      <c r="AG13" s="65"/>
+      <c r="AH13" s="65"/>
+      <c r="AI13" s="65"/>
+      <c r="AJ13" s="65"/>
+      <c r="AK13" s="65"/>
+      <c r="AL13" s="65"/>
+      <c r="AM13" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="62"/>
-      <c r="R13" s="62"/>
-      <c r="S13" s="62"/>
-      <c r="T13" s="62"/>
-      <c r="U13" s="62"/>
-      <c r="V13" s="62"/>
-      <c r="W13" s="62"/>
-      <c r="X13" s="62"/>
-      <c r="Y13" s="62"/>
-      <c r="Z13" s="62"/>
-      <c r="AA13" s="62"/>
-      <c r="AB13" s="62"/>
-      <c r="AC13" s="62"/>
-      <c r="AD13" s="62"/>
-      <c r="AE13" s="62"/>
-      <c r="AF13" s="62"/>
-      <c r="AG13" s="62"/>
-      <c r="AH13" s="62"/>
-      <c r="AI13" s="62"/>
-      <c r="AJ13" s="62"/>
-      <c r="AK13" s="62"/>
-      <c r="AL13" s="62"/>
-      <c r="AM13" s="64" t="s">
+      <c r="AN13" s="65"/>
+      <c r="AO13" s="65"/>
+      <c r="AP13" s="65"/>
+      <c r="AQ13" s="65"/>
+      <c r="AR13" s="65"/>
+      <c r="AS13" s="65"/>
+      <c r="AT13" s="65"/>
+      <c r="AU13" s="65"/>
+      <c r="AV13" s="65"/>
+      <c r="AW13" s="65"/>
+      <c r="AX13" s="65"/>
+      <c r="AY13" s="65"/>
+      <c r="AZ13" s="65"/>
+      <c r="BA13" s="65"/>
+      <c r="BB13" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="AN13" s="62"/>
-      <c r="AO13" s="62"/>
-      <c r="AP13" s="62"/>
-      <c r="AQ13" s="62"/>
-      <c r="AR13" s="62"/>
-      <c r="AS13" s="62"/>
-      <c r="AT13" s="62"/>
-      <c r="AU13" s="62"/>
-      <c r="AV13" s="62"/>
-      <c r="AW13" s="62"/>
-      <c r="AX13" s="62"/>
-      <c r="AY13" s="62"/>
-      <c r="AZ13" s="62"/>
-      <c r="BA13" s="62"/>
-      <c r="BB13" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC13" s="62"/>
-      <c r="BD13" s="62"/>
-      <c r="BE13" s="62"/>
-      <c r="BF13" s="62"/>
-      <c r="BG13" s="62"/>
-      <c r="BH13" s="62"/>
-      <c r="BI13" s="62"/>
-      <c r="BJ13" s="62"/>
-      <c r="BK13" s="62"/>
-      <c r="BL13" s="62"/>
-      <c r="BM13" s="62"/>
-      <c r="BN13" s="62"/>
-      <c r="BO13" s="62"/>
-      <c r="BP13" s="62"/>
-      <c r="BQ13" s="62"/>
-      <c r="BR13" s="62"/>
-      <c r="BS13" s="62"/>
-      <c r="BT13" s="62"/>
-      <c r="BU13" s="62"/>
-      <c r="BV13" s="62"/>
-      <c r="BW13" s="62"/>
-      <c r="BX13" s="62"/>
-      <c r="BY13" s="62"/>
-      <c r="BZ13" s="62"/>
-      <c r="CA13" s="62"/>
-      <c r="CB13" s="62"/>
-      <c r="CC13" s="62"/>
-      <c r="CD13" s="62"/>
-      <c r="CE13" s="62"/>
+      <c r="BC13" s="65"/>
+      <c r="BD13" s="65"/>
+      <c r="BE13" s="65"/>
+      <c r="BF13" s="65"/>
+      <c r="BG13" s="65"/>
+      <c r="BH13" s="65"/>
+      <c r="BI13" s="65"/>
+      <c r="BJ13" s="65"/>
+      <c r="BK13" s="65"/>
+      <c r="BL13" s="65"/>
+      <c r="BM13" s="65"/>
+      <c r="BN13" s="65"/>
+      <c r="BO13" s="65"/>
+      <c r="BP13" s="65"/>
+      <c r="BQ13" s="65"/>
+      <c r="BR13" s="65"/>
+      <c r="BS13" s="65"/>
+      <c r="BT13" s="65"/>
+      <c r="BU13" s="65"/>
+      <c r="BV13" s="65"/>
+      <c r="BW13" s="65"/>
+      <c r="BX13" s="65"/>
+      <c r="BY13" s="65"/>
+      <c r="BZ13" s="65"/>
+      <c r="CA13" s="65"/>
+      <c r="CB13" s="65"/>
+      <c r="CC13" s="65"/>
+      <c r="CD13" s="65"/>
+      <c r="CE13" s="65"/>
     </row>
     <row r="14" spans="1:83" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="19"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="61" t="s">
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="62"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="63" t="s">
+      <c r="O14" s="65"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="O14" s="62"/>
-      <c r="P14" s="62"/>
-      <c r="Q14" s="62"/>
-      <c r="R14" s="62"/>
-      <c r="S14" s="61" t="s">
+      <c r="T14" s="65"/>
+      <c r="U14" s="65"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="T14" s="62"/>
-      <c r="U14" s="62"/>
-      <c r="V14" s="62"/>
-      <c r="W14" s="62"/>
-      <c r="X14" s="63" t="s">
+      <c r="Y14" s="65"/>
+      <c r="Z14" s="65"/>
+      <c r="AA14" s="65"/>
+      <c r="AB14" s="65"/>
+      <c r="AC14" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="Y14" s="62"/>
-      <c r="Z14" s="62"/>
-      <c r="AA14" s="62"/>
-      <c r="AB14" s="62"/>
-      <c r="AC14" s="61" t="s">
+      <c r="AD14" s="65"/>
+      <c r="AE14" s="65"/>
+      <c r="AF14" s="65"/>
+      <c r="AG14" s="65"/>
+      <c r="AH14" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="AD14" s="62"/>
-      <c r="AE14" s="62"/>
-      <c r="AF14" s="62"/>
-      <c r="AG14" s="62"/>
-      <c r="AH14" s="63" t="s">
+      <c r="AI14" s="65"/>
+      <c r="AJ14" s="65"/>
+      <c r="AK14" s="65"/>
+      <c r="AL14" s="65"/>
+      <c r="AM14" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="AI14" s="62"/>
-      <c r="AJ14" s="62"/>
-      <c r="AK14" s="62"/>
-      <c r="AL14" s="62"/>
-      <c r="AM14" s="61" t="s">
+      <c r="AN14" s="65"/>
+      <c r="AO14" s="65"/>
+      <c r="AP14" s="65"/>
+      <c r="AQ14" s="65"/>
+      <c r="AR14" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="AN14" s="62"/>
-      <c r="AO14" s="62"/>
-      <c r="AP14" s="62"/>
-      <c r="AQ14" s="62"/>
-      <c r="AR14" s="63" t="s">
+      <c r="AS14" s="65"/>
+      <c r="AT14" s="65"/>
+      <c r="AU14" s="65"/>
+      <c r="AV14" s="65"/>
+      <c r="AW14" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="AS14" s="62"/>
-      <c r="AT14" s="62"/>
-      <c r="AU14" s="62"/>
-      <c r="AV14" s="62"/>
-      <c r="AW14" s="61" t="s">
+      <c r="AX14" s="65"/>
+      <c r="AY14" s="65"/>
+      <c r="AZ14" s="65"/>
+      <c r="BA14" s="65"/>
+      <c r="BB14" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="AX14" s="62"/>
-      <c r="AY14" s="62"/>
-      <c r="AZ14" s="62"/>
-      <c r="BA14" s="62"/>
-      <c r="BB14" s="63" t="s">
+      <c r="BC14" s="65"/>
+      <c r="BD14" s="65"/>
+      <c r="BE14" s="65"/>
+      <c r="BF14" s="65"/>
+      <c r="BG14" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="BC14" s="62"/>
-      <c r="BD14" s="62"/>
-      <c r="BE14" s="62"/>
-      <c r="BF14" s="62"/>
-      <c r="BG14" s="61" t="s">
+      <c r="BH14" s="65"/>
+      <c r="BI14" s="65"/>
+      <c r="BJ14" s="65"/>
+      <c r="BK14" s="65"/>
+      <c r="BL14" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="BH14" s="62"/>
-      <c r="BI14" s="62"/>
-      <c r="BJ14" s="62"/>
-      <c r="BK14" s="62"/>
-      <c r="BL14" s="63" t="s">
+      <c r="BM14" s="65"/>
+      <c r="BN14" s="65"/>
+      <c r="BO14" s="65"/>
+      <c r="BP14" s="65"/>
+      <c r="BQ14" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="BM14" s="62"/>
-      <c r="BN14" s="62"/>
-      <c r="BO14" s="62"/>
-      <c r="BP14" s="62"/>
-      <c r="BQ14" s="61" t="s">
+      <c r="BR14" s="65"/>
+      <c r="BS14" s="65"/>
+      <c r="BT14" s="65"/>
+      <c r="BU14" s="65"/>
+      <c r="BV14" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="BR14" s="62"/>
-      <c r="BS14" s="62"/>
-      <c r="BT14" s="62"/>
-      <c r="BU14" s="62"/>
-      <c r="BV14" s="63" t="s">
+      <c r="BW14" s="65"/>
+      <c r="BX14" s="65"/>
+      <c r="BY14" s="65"/>
+      <c r="BZ14" s="65"/>
+      <c r="CA14" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="BW14" s="62"/>
-      <c r="BX14" s="62"/>
-      <c r="BY14" s="62"/>
-      <c r="BZ14" s="62"/>
-      <c r="CA14" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="CB14" s="62"/>
-      <c r="CC14" s="62"/>
-      <c r="CD14" s="62"/>
-      <c r="CE14" s="62"/>
+      <c r="CB14" s="65"/>
+      <c r="CC14" s="65"/>
+      <c r="CD14" s="65"/>
+      <c r="CE14" s="65"/>
     </row>
     <row r="15" spans="1:83" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="19"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
       <c r="I15" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
@@ -2057,7 +2090,7 @@
       <c r="AD15" s="21"/>
       <c r="AE15" s="22"/>
       <c r="AF15" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AG15" s="21"/>
       <c r="AH15" s="21"/>
@@ -2081,7 +2114,7 @@
       <c r="AZ15" s="21"/>
       <c r="BA15" s="22"/>
       <c r="BB15" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BC15" s="21"/>
       <c r="BD15" s="21"/>
@@ -2104,7 +2137,7 @@
       <c r="BU15" s="21"/>
       <c r="BV15" s="22"/>
       <c r="BW15" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BX15" s="21"/>
       <c r="BY15" s="21"/>
@@ -2117,237 +2150,237 @@
     </row>
     <row r="16" spans="1:83" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="19"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
       <c r="I16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="K16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="L16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="M16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="N16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="P16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="P16" s="23" t="s">
+      <c r="Q16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="23" t="s">
+      <c r="R16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="R16" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="S16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="T16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="T16" s="23" t="s">
+      <c r="U16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="U16" s="23" t="s">
+      <c r="V16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="V16" s="23" t="s">
+      <c r="W16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="W16" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="X16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="Y16" s="23" t="s">
+      <c r="Z16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="Z16" s="23" t="s">
+      <c r="AA16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="AA16" s="23" t="s">
+      <c r="AB16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="AB16" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="AC16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AD16" s="23" t="s">
+      <c r="AE16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AE16" s="23" t="s">
+      <c r="AF16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="AF16" s="23" t="s">
+      <c r="AG16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="AG16" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="AH16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AI16" s="23" t="s">
+      <c r="AJ16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AJ16" s="23" t="s">
+      <c r="AK16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="AK16" s="23" t="s">
+      <c r="AL16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="AL16" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="AM16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AN16" s="24" t="s">
+      <c r="AO16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AO16" s="24" t="s">
+      <c r="AP16" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AP16" s="24" t="s">
+      <c r="AQ16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AQ16" s="24" t="s">
-        <v>40</v>
-      </c>
       <c r="AR16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="AS16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AS16" s="24" t="s">
+      <c r="AT16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AT16" s="24" t="s">
+      <c r="AU16" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AU16" s="24" t="s">
+      <c r="AV16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AV16" s="24" t="s">
-        <v>40</v>
-      </c>
       <c r="AW16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AX16" s="24" t="s">
+      <c r="AY16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AY16" s="24" t="s">
+      <c r="AZ16" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AZ16" s="24" t="s">
+      <c r="BA16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="BA16" s="24" t="s">
-        <v>40</v>
-      </c>
       <c r="BB16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="BC16" s="25" t="s">
+      <c r="BD16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="BD16" s="25" t="s">
+      <c r="BE16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="BE16" s="25" t="s">
+      <c r="BF16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="BF16" s="25" t="s">
-        <v>40</v>
-      </c>
       <c r="BG16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="BH16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="BH16" s="25" t="s">
+      <c r="BI16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="BI16" s="25" t="s">
+      <c r="BJ16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="BJ16" s="25" t="s">
+      <c r="BK16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="BK16" s="25" t="s">
-        <v>40</v>
-      </c>
       <c r="BL16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="BM16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="BM16" s="25" t="s">
+      <c r="BN16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="BN16" s="25" t="s">
+      <c r="BO16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="BO16" s="25" t="s">
+      <c r="BP16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="BP16" s="25" t="s">
-        <v>40</v>
-      </c>
       <c r="BQ16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="BR16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="BR16" s="25" t="s">
+      <c r="BS16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="BS16" s="25" t="s">
+      <c r="BT16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="BT16" s="25" t="s">
+      <c r="BU16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="BU16" s="25" t="s">
-        <v>40</v>
-      </c>
       <c r="BV16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="BW16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="BW16" s="25" t="s">
+      <c r="BX16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="BX16" s="25" t="s">
+      <c r="BY16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="BY16" s="25" t="s">
+      <c r="BZ16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="BZ16" s="25" t="s">
-        <v>40</v>
-      </c>
       <c r="CA16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="CB16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="CB16" s="25" t="s">
+      <c r="CC16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="CC16" s="25" t="s">
+      <c r="CD16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="CD16" s="25" t="s">
+      <c r="CE16" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="CE16" s="25" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:83" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -2356,7 +2389,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
@@ -2595,16 +2628,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="80" t="s">
+      <c r="E18" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="63" t="s">
         <v>67</v>
-      </c>
-      <c r="F18" s="80" t="s">
-        <v>68</v>
       </c>
       <c r="G18" s="35">
         <v>10</v>
@@ -2694,16 +2727,16 @@
         <v>1.2</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="36" t="s">
         <v>43</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>44</v>
       </c>
       <c r="G19" s="35">
         <v>10</v>
@@ -2793,16 +2826,16 @@
         <v>1.3</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="63" t="s">
         <v>69</v>
-      </c>
-      <c r="F20" s="80" t="s">
-        <v>70</v>
       </c>
       <c r="G20" s="35">
         <v>10</v>
@@ -2892,7 +2925,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="44"/>
       <c r="E21" s="45"/>
@@ -2981,16 +3014,16 @@
         <v>2.1</v>
       </c>
       <c r="C22" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="E22" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="F22" s="36" t="s">
         <v>47</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>48</v>
       </c>
       <c r="G22" s="35">
         <v>3</v>
@@ -3080,19 +3113,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="80" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="80" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="80" t="s">
-        <v>77</v>
+      <c r="G23" s="63" t="s">
+        <v>76</v>
       </c>
       <c r="H23" s="54">
         <v>0</v>
@@ -3178,17 +3211,17 @@
       <c r="B24" s="33">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C24" s="78" t="s">
-        <v>61</v>
+      <c r="C24" s="61" t="s">
+        <v>60</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>50</v>
       </c>
       <c r="G24" s="35">
         <v>10</v>
@@ -3278,7 +3311,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D25" s="44"/>
       <c r="E25" s="45"/>
@@ -3367,16 +3400,16 @@
         <v>3.1</v>
       </c>
       <c r="C26" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="79" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="D26" s="62" t="s">
+        <v>63</v>
       </c>
       <c r="E26" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="80" t="s">
-        <v>73</v>
+        <v>51</v>
+      </c>
+      <c r="F26" s="63" t="s">
+        <v>72</v>
       </c>
       <c r="G26" s="35">
         <v>10</v>
@@ -3466,16 +3499,16 @@
         <v>3.2</v>
       </c>
       <c r="C27" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="36" t="s">
         <v>53</v>
-      </c>
-      <c r="D27" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="80" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="36" t="s">
-        <v>54</v>
       </c>
       <c r="G27" s="35">
         <v>10</v>
@@ -3565,16 +3598,16 @@
         <v>3.3</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="63" t="s">
         <v>75</v>
-      </c>
-      <c r="F28" s="80" t="s">
-        <v>76</v>
       </c>
       <c r="G28" s="35">
         <v>10</v>
@@ -4605,18 +4638,14 @@
     <row r="973" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="S7:W7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="N9:W9"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="G13:G16"/>
-    <mergeCell ref="H13:H16"/>
-    <mergeCell ref="I13:AL13"/>
+    <mergeCell ref="CA14:CE14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="X14:AB14"/>
+    <mergeCell ref="AC14:AG14"/>
+    <mergeCell ref="AH14:AL14"/>
+    <mergeCell ref="AM14:AQ14"/>
+    <mergeCell ref="AR14:AV14"/>
     <mergeCell ref="AM13:BA13"/>
     <mergeCell ref="BB13:CE13"/>
     <mergeCell ref="B10:C10"/>
@@ -4633,14 +4662,18 @@
     <mergeCell ref="BL14:BP14"/>
     <mergeCell ref="BQ14:BU14"/>
     <mergeCell ref="BV14:BZ14"/>
-    <mergeCell ref="CA14:CE14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="AC14:AG14"/>
-    <mergeCell ref="AH14:AL14"/>
-    <mergeCell ref="AM14:AQ14"/>
-    <mergeCell ref="AR14:AV14"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="H13:H16"/>
+    <mergeCell ref="I13:AL13"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="S7:W7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="N9:W9"/>
   </mergeCells>
   <conditionalFormatting sqref="H18:H20 H22:H28">
     <cfRule type="colorScale" priority="1">

</xml_diff>